<commit_message>
Modifica grafico waiting time over response time
</commit_message>
<xml_diff>
--- a/analysis/waitingTimeOverResponseTime/WaitingTime over Response Time Clarissa Ennesimo.xlsx
+++ b/analysis/waitingTimeOverResponseTime/WaitingTime over Response Time Clarissa Ennesimo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clari\Desktop\Git\PECSNproject\analysis\waitingTimeOverResponseTime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F173A9BC-ACA3-414D-BD36-03AEA1AC42BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462BCEC4-D956-4A19-9B93-08BBCD2ABCAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{538F4401-FBAF-45AE-BC34-26D4C2B91D12}"/>
   </bookViews>
@@ -679,7 +679,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -689,6 +693,21 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -853,10 +872,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -878,13 +899,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Percentuale" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="42">
     <dxf>
@@ -3399,779 +3426,6 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Waiting time over response time</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.38081745846797355"/>
-          <c:y val="2.3170087599350873E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="5.7065436379753927E-2"/>
-          <c:y val="8.7872648441355519E-2"/>
-          <c:w val="0.90229157229608459"/>
-          <c:h val="0.80268097982104303"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tutto!$B$63</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>responseTime</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Tutto!$A$64:$A$96</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>(Tutto!$A$64:$A$68,Tutto!$A$71:$A$75,Tutto!$A$78:$A$82,Tutto!$A$85:$A$89,Tutto!$A$92:$A$96)</c:f>
-              <c:strCache>
-                <c:ptCount val="23"/>
-                <c:pt idx="3">
-                  <c:v>9ms</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10ms</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13ms</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>15ms</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>20ms</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Tutto!$B$64:$B$97</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>(Tutto!$B$64:$B$68,Tutto!$B$71:$B$75,Tutto!$B$78:$B$82,Tutto!$B$85:$B$89,Tutto!$B$92:$B$96)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
-                <c:pt idx="0">
-                  <c:v>2.8067130090194001E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0406116702319999E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.7807900061059E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.6987447527817001E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.51000924151E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.6947130723938E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.8032723235759E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.6176626114815001E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.4533592185962001E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.4147296596155001E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.6203654808635998E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.6218137262323001E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.3886128191140001E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.2449959588957E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.1801207307661E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.5445008520897001E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.5449856236502999E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.3596242982112001E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.2099763227775E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.1430084021359E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.3498276030079E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.4314519690025999E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.2357299559384E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.1033287938354E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.0279859875525E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:categoryFilterExceptions>
-                <c15:categoryFilterException>
-                  <c15:sqref>Tutto!$B$70</c15:sqref>
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:solidFill>
-                      <a:schemeClr val="accent6"/>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:solidFill>
-                        <a:schemeClr val="accent1"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c15:spPr>
-                  <c15:invertIfNegative val="0"/>
-                  <c15:bubble3D val="0"/>
-                </c15:categoryFilterException>
-                <c15:categoryFilterException>
-                  <c15:sqref>Tutto!$B$77</c15:sqref>
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:solidFill>
-                      <a:schemeClr val="accent6"/>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c15:spPr>
-                  <c15:invertIfNegative val="0"/>
-                  <c15:bubble3D val="0"/>
-                </c15:categoryFilterException>
-                <c15:categoryFilterException>
-                  <c15:sqref>Tutto!$B$84</c15:sqref>
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:solidFill>
-                      <a:schemeClr val="accent6"/>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c15:spPr>
-                  <c15:invertIfNegative val="0"/>
-                  <c15:bubble3D val="0"/>
-                </c15:categoryFilterException>
-                <c15:categoryFilterException>
-                  <c15:sqref>Tutto!$B$91</c15:sqref>
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:solidFill>
-                      <a:schemeClr val="accent6"/>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c15:spPr>
-                  <c15:invertIfNegative val="0"/>
-                  <c15:bubble3D val="0"/>
-                </c15:categoryFilterException>
-                <c15:categoryFilterException>
-                  <c15:sqref>Tutto!$B$97</c15:sqref>
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:solidFill>
-                      <a:schemeClr val="accent6"/>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c15:spPr>
-                  <c15:invertIfNegative val="0"/>
-                  <c15:bubble3D val="0"/>
-                </c15:categoryFilterException>
-              </c15:categoryFilterExceptions>
-            </c:ext>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7B17-4ECA-BD3C-522B401A3136}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tutto!$C$63</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>waitingTime</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Tutto!$A$64:$A$96</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>(Tutto!$A$64:$A$68,Tutto!$A$71:$A$75,Tutto!$A$78:$A$82,Tutto!$A$85:$A$89,Tutto!$A$92:$A$96)</c:f>
-              <c:strCache>
-                <c:ptCount val="23"/>
-                <c:pt idx="3">
-                  <c:v>9ms</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10ms</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13ms</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>15ms</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>20ms</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Tutto!$C$64:$C$97</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>(Tutto!$C$64:$C$68,Tutto!$C$71:$C$75,Tutto!$C$78:$C$82,Tutto!$C$85:$C$89,Tutto!$C$92:$C$96)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
-                <c:pt idx="0">
-                  <c:v>2.0837669212819002E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.3160471373677001E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0548444963124E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.6994320127142004E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.7467192152897999E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.9715960667489998E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0786049510818E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.9169827750461006E-3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7.2451393820031004E-3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6.7924577139844003E-3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.897270108735E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8.9724953134429995E-3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6.6255765369497999E-3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5.1588666916589001E-3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4.4418071915590003E-3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.8213578131681001E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8.2033069719258996E-3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>6.3356192942134997E-3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4.8092587587292004E-3</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>4.0746928203527003E-3</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.6267183583888001E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>7.069475965771E-3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>5.0972478953318001E-3</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3.7446506577407E-3</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2.9223895046124999E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:categoryFilterExceptions>
-                <c15:categoryFilterException>
-                  <c15:sqref>Tutto!$C$70</c15:sqref>
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:solidFill>
-                      <a:schemeClr val="accent6">
-                        <a:lumMod val="40000"/>
-                        <a:lumOff val="60000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c15:spPr>
-                  <c15:invertIfNegative val="0"/>
-                  <c15:bubble3D val="0"/>
-                </c15:categoryFilterException>
-                <c15:categoryFilterException>
-                  <c15:sqref>Tutto!$C$77</c15:sqref>
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:solidFill>
-                      <a:schemeClr val="accent6">
-                        <a:lumMod val="40000"/>
-                        <a:lumOff val="60000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c15:spPr>
-                  <c15:invertIfNegative val="0"/>
-                  <c15:bubble3D val="0"/>
-                </c15:categoryFilterException>
-                <c15:categoryFilterException>
-                  <c15:sqref>Tutto!$C$84</c15:sqref>
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:solidFill>
-                      <a:schemeClr val="accent6">
-                        <a:lumMod val="40000"/>
-                        <a:lumOff val="60000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c15:spPr>
-                  <c15:invertIfNegative val="0"/>
-                  <c15:bubble3D val="0"/>
-                </c15:categoryFilterException>
-                <c15:categoryFilterException>
-                  <c15:sqref>Tutto!$C$91</c15:sqref>
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:solidFill>
-                      <a:schemeClr val="accent6">
-                        <a:lumMod val="40000"/>
-                        <a:lumOff val="60000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c15:spPr>
-                  <c15:invertIfNegative val="0"/>
-                  <c15:bubble3D val="0"/>
-                </c15:categoryFilterException>
-                <c15:categoryFilterException>
-                  <c15:sqref>Tutto!$C$97</c15:sqref>
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:solidFill>
-                      <a:schemeClr val="accent6">
-                        <a:lumMod val="40000"/>
-                        <a:lumOff val="60000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c15:spPr>
-                  <c15:invertIfNegative val="0"/>
-                  <c15:bubble3D val="0"/>
-                </c15:categoryFilterException>
-              </c15:categoryFilterExceptions>
-            </c:ext>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7B17-4ECA-BD3C-522B401A3136}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="100"/>
-        <c:axId val="1928805952"/>
-        <c:axId val="1928813856"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1928805952"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1928813856"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:tickLblSkip val="1"/>
-        <c:tickMarkSkip val="7"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1928813856"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1928805952"/>
-        <c:crossesAt val="1"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
               <a:t>Non monitoring</a:t>
             </a:r>
           </a:p>
@@ -4576,7 +3830,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
@@ -5319,6 +4573,1810 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Waiting time over response time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.3787480212680131"/>
+          <c:y val="4.5996277129951177E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.3941849212984269E-2"/>
+          <c:y val="0.12164890271989987"/>
+          <c:w val="0.88884001270038571"/>
+          <c:h val="0.73927508079498716"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tutto!$B$63</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>responseTime</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tutto!$A$64:$A$96</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Tutto!$A$64:$A$68,Tutto!$A$71:$A$75,Tutto!$A$78:$A$82,Tutto!$A$85:$A$89,Tutto!$A$92:$A$96)</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="3">
+                  <c:v>9ms</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10ms</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13ms</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15ms</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20ms</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tutto!$B$64:$B$97</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Tutto!$B$64:$B$68,Tutto!$B$71:$B$75,Tutto!$B$78:$B$82,Tutto!$B$85:$B$89,Tutto!$B$92:$B$96)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>2.8067130090194001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0406116702319999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7807900061059E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6987447527817001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.51000924151E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6947130723938E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8032723235759E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6176626114815001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4533592185962001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4147296596155001E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.6203654808635998E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6218137262323001E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3886128191140001E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2449959588957E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1801207307661E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.5445008520897001E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.5449856236502999E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.3596242982112001E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2099763227775E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.1430084021359E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.3498276030079E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.4314519690025999E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.2357299559384E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.1033287938354E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.0279859875525E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:categoryFilterExceptions>
+                <c15:categoryFilterException>
+                  <c15:sqref>Tutto!$B$70</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+                <c15:categoryFilterException>
+                  <c15:sqref>Tutto!$B$77</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+                <c15:categoryFilterException>
+                  <c15:sqref>Tutto!$B$84</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+                <c15:categoryFilterException>
+                  <c15:sqref>Tutto!$B$91</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+                <c15:categoryFilterException>
+                  <c15:sqref>Tutto!$B$97</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+              </c15:categoryFilterExceptions>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5742-47AE-B538-E330662DBD2D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tutto!$C$63</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>waitingTime</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{EE378DD6-4E5E-4748-9B03-1AFE27D6FFED}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000018-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{9A5AC313-D73A-4A3B-8EEF-A05A858B114E}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000019-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{92131120-DE92-4545-BA45-E7DD44465BF8}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001A-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{6BF4C4BE-C463-4CF1-BE6B-ECEBC7E35D72}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001B-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{F480CCB7-E6DC-4FCF-B595-D6D557034AEA}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001C-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{DE605FBC-EC42-4F15-98CB-B828C80085A1}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001E-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{4C0CC767-6BA8-4ACA-89FA-5D87921D7D6B}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001F-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{4A36CEF7-FB4B-47B4-A844-3910BACCAFEC}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000020-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{9A4A8726-5AEA-453D-B7BC-B40D79F26C37}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000021-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{9957A737-4B96-46DB-A33E-DFAE9CD859E0}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000022-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{A83F9458-27EF-48F6-A296-9B55164B8632}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000024-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{25287519-9EA9-47BE-85BB-F1290445C087}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000025-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{A07ACB7D-175A-4D2B-8670-FE140372B489}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000026-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{714E6694-A3A5-4AE4-BFFF-F85209BB7C54}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000027-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{2BFF02AE-86A3-4142-9368-1FBDFDABE99D}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000028-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{93AC3636-735E-4242-B088-7361522DFA64}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000002A-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{28249DF2-F42A-4777-876C-F64A186C18F7}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000002B-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{FB1C4664-E2A2-44D6-8023-C795F234742D}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000002C-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{FC0CCFB9-0793-4331-80D6-986B5273ED65}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000002D-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{892A0649-173E-48EE-9C96-95205BBDBF91}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000002E-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="20"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{AF8134F0-E56D-4992-A37D-8AB0CD15BC32}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000030-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="21"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{B8B62B6F-2D1E-464B-8C37-C389798D6F4D}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000031-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="22"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{16504343-A353-467A-9C0F-4B84A9D96931}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000032-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="23"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{5DB25CE6-22E1-4C04-B2B3-B17EC14B731D}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000033-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="24"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{02A19934-A076-4850-B791-617AF762BF68}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[INTERVALLOCELLE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000034-5742-47AE-B538-E330662DBD2D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="0"/>
+                      <a:lumOff val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="35000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="0"/>
+                      <a:lumOff val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:path path="circle">
+                  <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+                </a:path>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="18000" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tutto!$A$64:$A$96</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Tutto!$A$64:$A$68,Tutto!$A$71:$A$75,Tutto!$A$78:$A$82,Tutto!$A$85:$A$89,Tutto!$A$92:$A$96)</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="3">
+                  <c:v>9ms</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10ms</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13ms</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15ms</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20ms</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tutto!$C$64:$C$97</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Tutto!$C$64:$C$68,Tutto!$C$71:$C$75,Tutto!$C$78:$C$82,Tutto!$C$85:$C$89,Tutto!$C$92:$C$96)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>2.0837669212819002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3160471373677001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0548444963124E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6994320127142004E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.7467192152897999E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9715960667489998E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0786049510818E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.9169827750461006E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.2451393820031004E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.7924577139844003E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.897270108735E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.9724953134429995E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.6255765369497999E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.1588666916589001E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.4418071915590003E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.8213578131681001E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.2033069719258996E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.3356192942134997E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.8092587587292004E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.0746928203527003E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.6267183583888001E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.069475965771E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.0972478953318001E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.7446506577407E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.9223895046124999E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>Tutto!$I$183:$I$215</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="33"/>
+                  <c:pt idx="0">
+                    <c:v>74,2%</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>64,5%</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>59,2%</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>57,1%</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>51,3%</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0,0%</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0,0%</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>73,2%</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>59,8%</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>55,1%</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>49,9%</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>48,0%</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>0,0%</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>0,0%</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>72,4%</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>55,3%</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>47,7%</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>41,4%</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>37,6%</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>0,0%</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>0,0%</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>71,6%</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>53,1%</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>46,6%</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>39,7%</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>35,6%</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
+                    <c:v>0,0%</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>0,0%</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
+                    <c:v>69,2%</c:v>
+                  </c:pt>
+                  <c:pt idx="29">
+                    <c:v>49,4%</c:v>
+                  </c:pt>
+                  <c:pt idx="30">
+                    <c:v>41,2%</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
+                    <c:v>33,9%</c:v>
+                  </c:pt>
+                  <c:pt idx="32">
+                    <c:v>28,4%</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:categoryFilterExceptions>
+                <c15:categoryFilterException>
+                  <c15:sqref>Tutto!$C$70</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6">
+                        <a:lumMod val="40000"/>
+                        <a:lumOff val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+                <c15:categoryFilterException>
+                  <c15:sqref>Tutto!$C$77</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6">
+                        <a:lumMod val="40000"/>
+                        <a:lumOff val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+                <c15:categoryFilterException>
+                  <c15:sqref>Tutto!$C$84</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6">
+                        <a:lumMod val="40000"/>
+                        <a:lumOff val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+                <c15:categoryFilterException>
+                  <c15:sqref>Tutto!$C$91</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6">
+                        <a:lumMod val="40000"/>
+                        <a:lumOff val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+                <c15:categoryFilterException>
+                  <c15:sqref>Tutto!$C$97</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6">
+                        <a:lumMod val="40000"/>
+                        <a:lumOff val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+              </c15:categoryFilterExceptions>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5742-47AE-B538-E330662DBD2D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="100"/>
+        <c:axId val="1928805952"/>
+        <c:axId val="1928813856"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1928805952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1928813856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="7"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1928813856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="92000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1928805952"/>
+        <c:crossesAt val="1"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -9204,16 +10262,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>14286</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>796835</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>679</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>375285</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>49529</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>517072</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9348,42 +10406,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>68036</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>242455</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>51955</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{115CA9CE-5368-4FE9-9360-3437A3FA46BD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
       <xdr:row>75</xdr:row>
@@ -9412,7 +10434,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9441,6 +10463,44 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>381001</xdr:colOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>163287</xdr:colOff>
+      <xdr:row>236</xdr:row>
+      <xdr:rowOff>136070</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD7257D9-AB9D-4163-84FB-2A8BB8DDEC43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -10226,8 +11286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65786636-41CC-4A4D-8137-86B7318C666B}">
   <dimension ref="A1:AM700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B53" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J151" sqref="J151"/>
+    <sheetView tabSelected="1" topLeftCell="B207" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S225" sqref="S225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10235,7 +11295,7 @@
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" customWidth="1"/>
     <col min="7" max="7" width="40.5703125" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.140625" customWidth="1"/>
@@ -15991,7 +17051,7 @@
       <c r="F151">
         <v>2.5962085008350001E-2</v>
       </c>
-      <c r="J151" s="22"/>
+      <c r="J151" s="21"/>
       <c r="K151" t="s">
         <v>80</v>
       </c>
@@ -16214,6 +17274,13 @@
       <c r="F154">
         <v>3.3686401011600003E-2</v>
       </c>
+      <c r="H154" s="24">
+        <v>74.239999999999995</v>
+      </c>
+      <c r="I154" s="23">
+        <f>H154/100</f>
+        <v>0.74239999999999995</v>
+      </c>
       <c r="K154" t="s">
         <v>80</v>
       </c>
@@ -16288,6 +17355,13 @@
       <c r="F155">
         <v>2.8163438654114002E-2</v>
       </c>
+      <c r="H155" s="24">
+        <v>64.492777169017998</v>
+      </c>
+      <c r="I155" s="23">
+        <f t="shared" ref="I155:J178" si="7">H155/100</f>
+        <v>0.64492777169018001</v>
+      </c>
       <c r="K155" t="s">
         <v>80</v>
       </c>
@@ -16362,6 +17436,13 @@
       <c r="F156">
         <v>3.1434591108909997E-2</v>
       </c>
+      <c r="H156" s="24">
+        <v>59.234637026016109</v>
+      </c>
+      <c r="I156" s="23">
+        <f t="shared" si="7"/>
+        <v>0.59234637026016113</v>
+      </c>
       <c r="K156" t="s">
         <v>80</v>
       </c>
@@ -16436,6 +17517,13 @@
       <c r="F157">
         <v>2.8994824797667001E-2</v>
       </c>
+      <c r="H157" s="24">
+        <v>57.097642225716072</v>
+      </c>
+      <c r="I157" s="23">
+        <f t="shared" si="7"/>
+        <v>0.57097642225716072</v>
+      </c>
       <c r="K157" t="s">
         <v>80</v>
       </c>
@@ -16510,6 +17598,13 @@
       <c r="F158">
         <v>3.1158199735143999E-2</v>
       </c>
+      <c r="H158" s="24">
+        <v>51.302462278595904</v>
+      </c>
+      <c r="I158" s="23">
+        <f t="shared" si="7"/>
+        <v>0.51302462278595906</v>
+      </c>
       <c r="K158" t="s">
         <v>80</v>
       </c>
@@ -16584,6 +17679,13 @@
       <c r="F159">
         <v>2.6179480191081E-2</v>
       </c>
+      <c r="H159" s="24">
+        <v>73.165343165740765</v>
+      </c>
+      <c r="I159" s="23">
+        <f t="shared" si="7"/>
+        <v>0.7316534316574077</v>
+      </c>
       <c r="K159" t="s">
         <v>80</v>
       </c>
@@ -16658,6 +17760,13 @@
       <c r="F160">
         <v>2.8292864278953E-2</v>
       </c>
+      <c r="H160" s="24">
+        <v>59.813758409097076</v>
+      </c>
+      <c r="I160" s="23">
+        <f t="shared" si="7"/>
+        <v>0.59813758409097073</v>
+      </c>
       <c r="K160" t="s">
         <v>80</v>
       </c>
@@ -16732,6 +17841,13 @@
       <c r="F161">
         <v>2.4628842957918E-2</v>
       </c>
+      <c r="H161" s="24">
+        <v>55.122636276297939</v>
+      </c>
+      <c r="I161" s="23">
+        <f t="shared" si="7"/>
+        <v>0.55122636276297943</v>
+      </c>
       <c r="K161" t="s">
         <v>80</v>
       </c>
@@ -16806,6 +17922,13 @@
       <c r="F162">
         <v>3.0747867017143E-2</v>
       </c>
+      <c r="H162" s="24">
+        <v>49.850988587674713</v>
+      </c>
+      <c r="I162" s="23">
+        <f t="shared" si="7"/>
+        <v>0.49850988587674716</v>
+      </c>
       <c r="K162" t="s">
         <v>80</v>
       </c>
@@ -16880,6 +18003,13 @@
       <c r="F163">
         <v>2.7870552785177E-2</v>
       </c>
+      <c r="H163" s="24">
+        <v>48.012407655540898</v>
+      </c>
+      <c r="I163" s="23">
+        <f t="shared" si="7"/>
+        <v>0.48012407655540895</v>
+      </c>
       <c r="K163" t="s">
         <v>80</v>
       </c>
@@ -16954,6 +18084,13 @@
       <c r="F164">
         <v>3.1437934761877999E-2</v>
       </c>
+      <c r="H164" s="24">
+        <v>72.404789430736685</v>
+      </c>
+      <c r="I164" s="23">
+        <f t="shared" si="7"/>
+        <v>0.72404789430736682</v>
+      </c>
       <c r="K164" t="s">
         <v>80</v>
       </c>
@@ -17028,6 +18165,13 @@
       <c r="F165">
         <v>3.1207769032286999E-2</v>
       </c>
+      <c r="H165" s="24">
+        <v>55.32383385536734</v>
+      </c>
+      <c r="I165" s="23">
+        <f t="shared" si="7"/>
+        <v>0.55323833855367344</v>
+      </c>
       <c r="K165" t="s">
         <v>80</v>
       </c>
@@ -17102,6 +18246,13 @@
       <c r="F166">
         <v>3.4621236868254003E-2</v>
       </c>
+      <c r="H166" s="24">
+        <v>47.71363511664272</v>
+      </c>
+      <c r="I166" s="23">
+        <f t="shared" si="7"/>
+        <v>0.47713635116642722</v>
+      </c>
       <c r="K166" t="s">
         <v>80</v>
       </c>
@@ -17176,6 +18327,13 @@
       <c r="F167">
         <v>2.6753438783676E-2</v>
       </c>
+      <c r="H167" s="24">
+        <v>41.436814752674117</v>
+      </c>
+      <c r="I167" s="23">
+        <f t="shared" si="7"/>
+        <v>0.41436814752674117</v>
+      </c>
       <c r="K167" t="s">
         <v>80</v>
       </c>
@@ -17250,6 +18408,13 @@
       <c r="F168">
         <v>3.3355517195132002E-2</v>
       </c>
+      <c r="H168" s="24">
+        <v>37.638582864954067</v>
+      </c>
+      <c r="I168" s="23">
+        <f t="shared" si="7"/>
+        <v>0.37638582864954068</v>
+      </c>
       <c r="K168" t="s">
         <v>80</v>
       </c>
@@ -17324,6 +18489,13 @@
       <c r="F169">
         <v>2.8977334199833001E-2</v>
       </c>
+      <c r="H169" s="25">
+        <v>71.580161259222592</v>
+      </c>
+      <c r="I169" s="23">
+        <f t="shared" si="7"/>
+        <v>0.71580161259222597</v>
+      </c>
       <c r="K169" t="s">
         <v>80</v>
       </c>
@@ -17398,6 +18570,13 @@
       <c r="F170">
         <v>3.3139074808059998E-2</v>
       </c>
+      <c r="H170" s="25">
+        <v>53.09633207164832</v>
+      </c>
+      <c r="I170" s="23">
+        <f t="shared" si="7"/>
+        <v>0.53096332071648322</v>
+      </c>
       <c r="K170" t="s">
         <v>80</v>
       </c>
@@ -17472,6 +18651,13 @@
       <c r="F171">
         <v>3.0803615399394E-2</v>
       </c>
+      <c r="H171" s="25">
+        <v>46.598308830969003</v>
+      </c>
+      <c r="I171" s="23">
+        <f t="shared" si="7"/>
+        <v>0.46598308830969004</v>
+      </c>
       <c r="K171" t="s">
         <v>80</v>
       </c>
@@ -17546,6 +18732,13 @@
       <c r="F172">
         <v>3.3257117368119003E-2</v>
       </c>
+      <c r="H172" s="25">
+        <v>39.746717916674186</v>
+      </c>
+      <c r="I172" s="23">
+        <f t="shared" si="7"/>
+        <v>0.39746717916674185</v>
+      </c>
       <c r="K172" t="s">
         <v>80</v>
       </c>
@@ -17620,6 +18813,13 @@
       <c r="F173">
         <v>2.824515533652E-2</v>
       </c>
+      <c r="H173" s="25">
+        <v>35.648843986959882</v>
+      </c>
+      <c r="I173" s="23">
+        <f t="shared" si="7"/>
+        <v>0.35648843986959883</v>
+      </c>
       <c r="K173" t="s">
         <v>80</v>
       </c>
@@ -17694,6 +18894,13 @@
       <c r="F174">
         <v>3.3212285365465999E-2</v>
       </c>
+      <c r="H174" s="25">
+        <v>69.227136335725945</v>
+      </c>
+      <c r="I174" s="23">
+        <f t="shared" si="7"/>
+        <v>0.69227136335725947</v>
+      </c>
       <c r="K174" t="s">
         <v>80</v>
       </c>
@@ -17768,6 +18975,13 @@
       <c r="F175">
         <v>3.3186570056390002E-2</v>
       </c>
+      <c r="H175" s="25">
+        <v>49.386749390528514</v>
+      </c>
+      <c r="I175" s="23">
+        <f t="shared" si="7"/>
+        <v>0.49386749390528517</v>
+      </c>
       <c r="K175" t="s">
         <v>80</v>
       </c>
@@ -17842,6 +19056,13 @@
       <c r="F176">
         <v>2.9437503545845001E-2</v>
       </c>
+      <c r="H176" s="25">
+        <v>41.248881851868724</v>
+      </c>
+      <c r="I176" s="23">
+        <f t="shared" si="7"/>
+        <v>0.41248881851868724</v>
+      </c>
       <c r="K176" t="s">
         <v>80</v>
       </c>
@@ -17916,6 +19137,13 @@
       <c r="F177">
         <v>2.6762159317224001E-2</v>
       </c>
+      <c r="H177" s="25">
+        <v>33.939571582497337</v>
+      </c>
+      <c r="I177" s="23">
+        <f t="shared" si="7"/>
+        <v>0.33939571582497335</v>
+      </c>
       <c r="K177" t="s">
         <v>80</v>
       </c>
@@ -17990,6 +19218,13 @@
       <c r="F178">
         <v>3.3943291719426998E-2</v>
       </c>
+      <c r="H178" s="25">
+        <v>28.428300969065994</v>
+      </c>
+      <c r="I178" s="23">
+        <f t="shared" si="7"/>
+        <v>0.28428300969065995</v>
+      </c>
       <c r="K178" t="s">
         <v>80</v>
       </c>
@@ -18360,6 +19595,12 @@
       <c r="F183">
         <v>3.2145040559848001E-2</v>
       </c>
+      <c r="H183" s="23">
+        <v>0.74239999999999995</v>
+      </c>
+      <c r="I183" s="23">
+        <v>0.74239999999999995</v>
+      </c>
       <c r="K183" t="s">
         <v>80</v>
       </c>
@@ -18434,6 +19675,12 @@
       <c r="F184">
         <v>3.1250350357663E-2</v>
       </c>
+      <c r="H184" s="23">
+        <v>0.64492777169018001</v>
+      </c>
+      <c r="I184" s="23">
+        <v>0.64492777169018001</v>
+      </c>
       <c r="K184" t="s">
         <v>80</v>
       </c>
@@ -18508,6 +19755,12 @@
       <c r="F185">
         <v>3.1205356194611001E-2</v>
       </c>
+      <c r="H185" s="23">
+        <v>0.59234637026016113</v>
+      </c>
+      <c r="I185" s="23">
+        <v>0.59234637026016113</v>
+      </c>
       <c r="K185" t="s">
         <v>80</v>
       </c>
@@ -18582,6 +19835,12 @@
       <c r="F186">
         <v>3.2815123648860002E-2</v>
       </c>
+      <c r="H186" s="23">
+        <v>0.57097642225716072</v>
+      </c>
+      <c r="I186" s="23">
+        <v>0.57097642225716072</v>
+      </c>
       <c r="K186" t="s">
         <v>80</v>
       </c>
@@ -18656,6 +19915,12 @@
       <c r="F187">
         <v>2.9287038881321999E-2</v>
       </c>
+      <c r="H187" s="23">
+        <v>0.51302462278595906</v>
+      </c>
+      <c r="I187" s="23">
+        <v>0.51302462278595906</v>
+      </c>
       <c r="K187" t="s">
         <v>80</v>
       </c>
@@ -18730,6 +19995,12 @@
       <c r="F188">
         <v>2.5913658224964001E-2</v>
       </c>
+      <c r="H188" s="23">
+        <v>0.7316534316574077</v>
+      </c>
+      <c r="I188" s="23">
+        <v>0</v>
+      </c>
       <c r="K188" t="s">
         <v>80</v>
       </c>
@@ -18804,6 +20075,12 @@
       <c r="F189">
         <v>3.0326439568946002E-2</v>
       </c>
+      <c r="H189" s="23">
+        <v>0.59813758409097073</v>
+      </c>
+      <c r="I189" s="23">
+        <v>0</v>
+      </c>
       <c r="K189" t="s">
         <v>80</v>
       </c>
@@ -18878,6 +20155,12 @@
       <c r="F190">
         <v>2.5961938792327999E-2</v>
       </c>
+      <c r="H190" s="23">
+        <v>0.55122636276297943</v>
+      </c>
+      <c r="I190" s="23">
+        <v>0.7316534316574077</v>
+      </c>
       <c r="K190" t="s">
         <v>80</v>
       </c>
@@ -18952,6 +20235,12 @@
       <c r="F191">
         <v>2.9748369389968998E-2</v>
       </c>
+      <c r="H191" s="23">
+        <v>0.49850988587674716</v>
+      </c>
+      <c r="I191" s="23">
+        <v>0.59813758409097073</v>
+      </c>
       <c r="K191" t="s">
         <v>80</v>
       </c>
@@ -19026,6 +20315,12 @@
       <c r="F192">
         <v>3.0553067680809998E-2</v>
       </c>
+      <c r="H192" s="23">
+        <v>0.48012407655540895</v>
+      </c>
+      <c r="I192" s="23">
+        <v>0.55122636276297943</v>
+      </c>
       <c r="K192" t="s">
         <v>80</v>
       </c>
@@ -19100,6 +20395,12 @@
       <c r="F193">
         <v>2.7844342069621001E-2</v>
       </c>
+      <c r="H193" s="23">
+        <v>0.72404789430736682</v>
+      </c>
+      <c r="I193" s="23">
+        <v>0.49850988587674716</v>
+      </c>
       <c r="K193" t="s">
         <v>80</v>
       </c>
@@ -19174,6 +20475,12 @@
       <c r="F194">
         <v>2.5545258431826E-2</v>
       </c>
+      <c r="H194" s="23">
+        <v>0.55323833855367344</v>
+      </c>
+      <c r="I194" s="23">
+        <v>0.48012407655540895</v>
+      </c>
       <c r="K194" t="s">
         <v>80</v>
       </c>
@@ -19248,6 +20555,12 @@
       <c r="F195">
         <v>3.1425898040578E-2</v>
       </c>
+      <c r="H195" s="23">
+        <v>0.47713635116642722</v>
+      </c>
+      <c r="I195" s="23">
+        <v>0</v>
+      </c>
       <c r="K195" t="s">
         <v>80</v>
       </c>
@@ -19322,6 +20635,12 @@
       <c r="F196">
         <v>2.5423009109199E-2</v>
       </c>
+      <c r="H196" s="23">
+        <v>0.41436814752674117</v>
+      </c>
+      <c r="I196" s="23">
+        <v>0</v>
+      </c>
       <c r="K196" t="s">
         <v>80</v>
       </c>
@@ -19396,6 +20715,12 @@
       <c r="F197">
         <v>3.0243802158186998E-2</v>
       </c>
+      <c r="H197" s="23">
+        <v>0.37638582864954068</v>
+      </c>
+      <c r="I197" s="23">
+        <v>0.72404789430736682</v>
+      </c>
       <c r="K197" t="s">
         <v>80</v>
       </c>
@@ -19470,6 +20795,12 @@
       <c r="F198">
         <v>3.1035551623486E-2</v>
       </c>
+      <c r="H198" s="23">
+        <v>0.71580161259222597</v>
+      </c>
+      <c r="I198" s="23">
+        <v>0.55323833855367344</v>
+      </c>
       <c r="K198" t="s">
         <v>80</v>
       </c>
@@ -19544,6 +20875,12 @@
       <c r="F199">
         <v>2.4489754596533998E-2</v>
       </c>
+      <c r="H199" s="23">
+        <v>0.53096332071648322</v>
+      </c>
+      <c r="I199" s="23">
+        <v>0.47713635116642722</v>
+      </c>
       <c r="K199" t="s">
         <v>80</v>
       </c>
@@ -19618,6 +20955,12 @@
       <c r="F200">
         <v>3.6446430399271E-2</v>
       </c>
+      <c r="H200" s="23">
+        <v>0.46598308830969004</v>
+      </c>
+      <c r="I200" s="23">
+        <v>0.41436814752674117</v>
+      </c>
       <c r="K200" t="s">
         <v>80</v>
       </c>
@@ -19692,6 +21035,12 @@
       <c r="F201">
         <v>1.3983937913947E-2</v>
       </c>
+      <c r="H201" s="23">
+        <v>0.39746717916674185</v>
+      </c>
+      <c r="I201" s="23">
+        <v>0.37638582864954068</v>
+      </c>
       <c r="K201" t="s">
         <v>80</v>
       </c>
@@ -19766,6 +21115,12 @@
       <c r="F202">
         <v>1.4748588242868999E-2</v>
       </c>
+      <c r="H202" s="23">
+        <v>0.35648843986959883</v>
+      </c>
+      <c r="I202" s="23">
+        <v>0</v>
+      </c>
       <c r="K202" t="s">
         <v>80</v>
       </c>
@@ -19840,6 +21195,12 @@
       <c r="F203">
         <v>1.4120430928911999E-2</v>
       </c>
+      <c r="H203" s="23">
+        <v>0.69227136335725903</v>
+      </c>
+      <c r="I203" s="23">
+        <v>0</v>
+      </c>
       <c r="K203" t="s">
         <v>80</v>
       </c>
@@ -19914,6 +21275,12 @@
       <c r="F204">
         <v>1.4202512548719E-2</v>
       </c>
+      <c r="H204" s="23">
+        <v>0.49386749390528517</v>
+      </c>
+      <c r="I204" s="23">
+        <v>0.71580161259222597</v>
+      </c>
       <c r="K204" t="s">
         <v>80</v>
       </c>
@@ -19988,6 +21355,12 @@
       <c r="F205">
         <v>1.432499221584E-2</v>
       </c>
+      <c r="H205" s="23">
+        <v>0.41248881851868724</v>
+      </c>
+      <c r="I205" s="23">
+        <v>0.53096332071648322</v>
+      </c>
       <c r="K205" t="s">
         <v>80</v>
       </c>
@@ -20062,6 +21435,12 @@
       <c r="F206">
         <v>1.4819883893603E-2</v>
       </c>
+      <c r="H206" s="23">
+        <v>0.33939571582497335</v>
+      </c>
+      <c r="I206" s="23">
+        <v>0.46598308830969004</v>
+      </c>
       <c r="K206" t="s">
         <v>80</v>
       </c>
@@ -20136,6 +21515,12 @@
       <c r="F207">
         <v>1.5180144487315E-2</v>
       </c>
+      <c r="H207" s="23">
+        <v>0.28428300969065995</v>
+      </c>
+      <c r="I207" s="23">
+        <v>0.39746717916674185</v>
+      </c>
       <c r="K207" t="s">
         <v>80</v>
       </c>
@@ -20210,6 +21595,9 @@
       <c r="F208">
         <v>1.540578714846E-2</v>
       </c>
+      <c r="I208" s="23">
+        <v>0.35648843986959883</v>
+      </c>
       <c r="K208" t="s">
         <v>80</v>
       </c>
@@ -20284,6 +21672,9 @@
       <c r="F209">
         <v>1.4941618304380001E-2</v>
       </c>
+      <c r="I209" s="23">
+        <v>0</v>
+      </c>
       <c r="K209" t="s">
         <v>80</v>
       </c>
@@ -20358,6 +21749,9 @@
       <c r="F210">
         <v>1.4751649879930001E-2</v>
       </c>
+      <c r="I210" s="23">
+        <v>0</v>
+      </c>
       <c r="K210" t="s">
         <v>80</v>
       </c>
@@ -20432,6 +21826,9 @@
       <c r="F211">
         <v>1.4540767114159E-2</v>
       </c>
+      <c r="I211" s="23">
+        <v>0.69227136335725903</v>
+      </c>
       <c r="K211" t="s">
         <v>80</v>
       </c>
@@ -20506,6 +21903,9 @@
       <c r="F212">
         <v>1.3817983944229E-2</v>
       </c>
+      <c r="I212" s="23">
+        <v>0.49386749390528517</v>
+      </c>
       <c r="K212" t="s">
         <v>80</v>
       </c>
@@ -20580,6 +21980,9 @@
       <c r="F213">
         <v>1.458191389691E-2</v>
       </c>
+      <c r="I213" s="23">
+        <v>0.41248881851868724</v>
+      </c>
       <c r="K213" t="s">
         <v>80</v>
       </c>
@@ -20654,6 +22057,10 @@
       <c r="F214">
         <v>1.453451417203E-2</v>
       </c>
+      <c r="G214" s="26"/>
+      <c r="I214" s="23">
+        <v>0.33939571582497335</v>
+      </c>
       <c r="K214" t="s">
         <v>80</v>
       </c>
@@ -20728,6 +22135,9 @@
       <c r="F215">
         <v>1.5713676297882999E-2</v>
       </c>
+      <c r="I215" s="23">
+        <v>0.28428300969065995</v>
+      </c>
       <c r="K215" t="s">
         <v>80</v>
       </c>
@@ -56075,6 +57485,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D64:D76 D78:D98">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D77">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -56086,8 +57508,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D77">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="H154:H178">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -56120,23 +57542,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E07C96B6-7598-4313-A645-4C802FD54B63}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="22"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="22" t="s">
         <v>193</v>
       </c>
-      <c r="B25" s="21"/>
+      <c r="B25" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>